<commit_message>
fix off-by-one feil, legg til noen produkter som ikke kom med, forbedre validering
</commit_message>
<xml_diff>
--- a/src/main/resources/deler.xlsx
+++ b/src/main/resources/deler.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://navno.sharepoint.com/sites/digihot/Shared Documents/Hugin/Deler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{843CC8DE-B14D-4FBC-9012-AC57BBF9DA88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB531656-5C1C-4F95-9E92-BE1E6F4ABC76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="500" windowWidth="35840" windowHeight="21240" firstSheet="1" xr2:uid="{BF3FA88B-012A-4523-8159-2DE03183410D}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="35840" windowHeight="21240" activeTab="1" xr2:uid="{BF3FA88B-012A-4523-8159-2DE03183410D}"/>
   </bookViews>
   <sheets>
     <sheet name="Deler (detaljer)" sheetId="5" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1589" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1590" uniqueCount="310">
   <si>
     <t>Navn</t>
   </si>
@@ -537,6 +537,9 @@
   </si>
   <si>
     <t>Cross 6 sb43 K</t>
+  </si>
+  <si>
+    <t>278337</t>
   </si>
   <si>
     <t>240199</t>
@@ -1556,8 +1559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D371AC0-AD41-4433-84FD-85875537ACF4}">
   <dimension ref="A1:I136"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15"/>
@@ -4426,8 +4429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0944327B-15A3-4968-91D3-16CF62ED0C05}">
   <dimension ref="A1:Z78"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.42578125" defaultRowHeight="15"/>
@@ -6082,6 +6085,9 @@
       <c r="A27" s="32" t="s">
         <v>164</v>
       </c>
+      <c r="B27" s="33" t="s">
+        <v>165</v>
+      </c>
       <c r="C27" s="28">
         <v>140928</v>
       </c>
@@ -6120,7 +6126,7 @@
         <v>220325</v>
       </c>
       <c r="P27" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="Q27" s="28">
         <v>181081</v>
@@ -6182,7 +6188,7 @@
         <v>220325</v>
       </c>
       <c r="P28" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="Q28" s="28">
         <v>181081</v>
@@ -6201,7 +6207,7 @@
     </row>
     <row r="29" spans="1:26" ht="15.95">
       <c r="A29" s="32" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B29" s="33">
         <v>317624</v>
@@ -6244,7 +6250,7 @@
         <v>220325</v>
       </c>
       <c r="P29" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="Q29" s="28">
         <v>181081</v>
@@ -6263,7 +6269,7 @@
     </row>
     <row r="30" spans="1:26" ht="15.95">
       <c r="A30" s="37" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B30" s="38">
         <v>326565</v>
@@ -6306,7 +6312,7 @@
         <v>220325</v>
       </c>
       <c r="P30" s="28" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="Q30" s="28">
         <v>181081</v>
@@ -6325,7 +6331,7 @@
     </row>
     <row r="31" spans="1:26" ht="15.95">
       <c r="A31" s="32" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B31" s="33">
         <v>278338</v>
@@ -6368,7 +6374,7 @@
         <v>220325</v>
       </c>
       <c r="P31" s="28" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="Q31" s="28">
         <v>181081</v>
@@ -6387,7 +6393,7 @@
     </row>
     <row r="32" spans="1:26" ht="15.95">
       <c r="A32" s="37" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B32" s="38">
         <v>326546</v>
@@ -6430,7 +6436,7 @@
         <v>220325</v>
       </c>
       <c r="P32" s="28" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="Q32" s="28">
         <v>181081</v>
@@ -6449,7 +6455,7 @@
     </row>
     <row r="33" spans="1:26" ht="15.95">
       <c r="A33" s="32" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B33" s="33">
         <v>317625</v>
@@ -6492,7 +6498,7 @@
         <v>220325</v>
       </c>
       <c r="P33" s="28" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="Q33" s="28">
         <v>181081</v>
@@ -6511,7 +6517,7 @@
     </row>
     <row r="34" spans="1:26" ht="15.95">
       <c r="A34" s="37" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B34" s="38">
         <v>326566</v>
@@ -6554,7 +6560,7 @@
         <v>220325</v>
       </c>
       <c r="P34" s="28" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="Q34" s="28">
         <v>181081</v>
@@ -6573,7 +6579,7 @@
     </row>
     <row r="35" spans="1:26" ht="15.95">
       <c r="A35" s="32" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B35" s="33">
         <v>278339</v>
@@ -6616,7 +6622,7 @@
         <v>220325</v>
       </c>
       <c r="P35" s="28" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="Q35" s="28">
         <v>181082</v>
@@ -6635,7 +6641,7 @@
     </row>
     <row r="36" spans="1:26" ht="15.95">
       <c r="A36" s="37" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B36" s="38">
         <v>326547</v>
@@ -6678,7 +6684,7 @@
         <v>220325</v>
       </c>
       <c r="P36" s="28" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="Q36" s="28">
         <v>181082</v>
@@ -6697,7 +6703,7 @@
     </row>
     <row r="37" spans="1:26" ht="15.95">
       <c r="A37" s="32" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B37" s="33">
         <v>317626</v>
@@ -6740,7 +6746,7 @@
         <v>220325</v>
       </c>
       <c r="P37" s="28" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="Q37" s="28">
         <v>181082</v>
@@ -6759,7 +6765,7 @@
     </row>
     <row r="38" spans="1:26" ht="15.95">
       <c r="A38" s="37" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B38" s="38">
         <v>326567</v>
@@ -6802,7 +6808,7 @@
         <v>220325</v>
       </c>
       <c r="P38" s="28" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="Q38" s="28">
         <v>181082</v>
@@ -6821,7 +6827,7 @@
     </row>
     <row r="39" spans="1:26" ht="15.95">
       <c r="A39" s="32" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B39" s="33">
         <v>278340</v>
@@ -6864,7 +6870,7 @@
         <v>220325</v>
       </c>
       <c r="P39" s="28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="Q39" s="28">
         <v>181082</v>
@@ -6883,7 +6889,7 @@
     </row>
     <row r="40" spans="1:26" ht="15.95">
       <c r="A40" s="37" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B40" s="38">
         <v>326548</v>
@@ -6926,7 +6932,7 @@
         <v>220325</v>
       </c>
       <c r="P40" s="28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="Q40" s="28">
         <v>181082</v>
@@ -6945,7 +6951,7 @@
     </row>
     <row r="41" spans="1:26" ht="15.95">
       <c r="A41" s="32" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B41" s="33">
         <v>317627</v>
@@ -6988,7 +6994,7 @@
         <v>220325</v>
       </c>
       <c r="P41" s="28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="Q41" s="28">
         <v>181082</v>
@@ -7007,7 +7013,7 @@
     </row>
     <row r="42" spans="1:26" ht="15.95">
       <c r="A42" s="37" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B42" s="38">
         <v>326568</v>
@@ -7050,7 +7056,7 @@
         <v>220325</v>
       </c>
       <c r="P42" s="28" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="Q42" s="28">
         <v>181082</v>
@@ -7069,7 +7075,7 @@
     </row>
     <row r="43" spans="1:26" ht="15.95">
       <c r="A43" s="37" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B43" s="38">
         <v>326527</v>
@@ -7114,7 +7120,7 @@
         <v>220325</v>
       </c>
       <c r="P43" s="28" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Q43" s="28">
         <v>181083</v>
@@ -7133,7 +7139,7 @@
     </row>
     <row r="44" spans="1:26" ht="15.95">
       <c r="A44" s="37" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B44" s="38">
         <v>326528</v>
@@ -7178,7 +7184,7 @@
         <v>220325</v>
       </c>
       <c r="P44" s="28" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="Q44" s="28">
         <v>181083</v>
@@ -7197,7 +7203,7 @@
     </row>
     <row r="45" spans="1:26" ht="15.95">
       <c r="A45" s="32" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B45" s="33">
         <v>278341</v>
@@ -7240,7 +7246,7 @@
         <v>220325</v>
       </c>
       <c r="P45" s="28" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Q45" s="28">
         <v>181083</v>
@@ -7259,7 +7265,7 @@
     </row>
     <row r="46" spans="1:26" ht="15.95">
       <c r="A46" s="37" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B46" s="38">
         <v>326549</v>
@@ -7302,7 +7308,7 @@
         <v>220325</v>
       </c>
       <c r="P46" s="28" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Q46" s="28">
         <v>181083</v>
@@ -7321,7 +7327,7 @@
     </row>
     <row r="47" spans="1:26" ht="15.95">
       <c r="A47" s="32" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B47" s="33">
         <v>317628</v>
@@ -7364,7 +7370,7 @@
         <v>220325</v>
       </c>
       <c r="P47" s="28" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Q47" s="28">
         <v>181083</v>
@@ -7383,7 +7389,7 @@
     </row>
     <row r="48" spans="1:26" ht="15.95">
       <c r="A48" s="37" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B48" s="38">
         <v>326569</v>
@@ -7426,7 +7432,7 @@
         <v>220325</v>
       </c>
       <c r="P48" s="28" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="Q48" s="28">
         <v>181083</v>
@@ -7445,7 +7451,7 @@
     </row>
     <row r="49" spans="1:26" ht="15.95">
       <c r="A49" s="32" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B49" s="33">
         <v>278342</v>
@@ -7488,7 +7494,7 @@
         <v>220325</v>
       </c>
       <c r="P49" s="28" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="Q49" s="28">
         <v>181083</v>
@@ -7507,7 +7513,7 @@
     </row>
     <row r="50" spans="1:26" ht="15.95">
       <c r="A50" s="37" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B50" s="38">
         <v>326550</v>
@@ -7550,7 +7556,7 @@
         <v>220325</v>
       </c>
       <c r="P50" s="28" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="Q50" s="28">
         <v>181083</v>
@@ -7569,7 +7575,7 @@
     </row>
     <row r="51" spans="1:26" ht="15.95">
       <c r="A51" s="32" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B51" s="33">
         <v>317629</v>
@@ -7612,7 +7618,7 @@
         <v>220325</v>
       </c>
       <c r="P51" s="28" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="Q51" s="28">
         <v>181083</v>
@@ -7631,7 +7637,7 @@
     </row>
     <row r="52" spans="1:26" ht="15.95">
       <c r="A52" s="37" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B52" s="38">
         <v>326570</v>
@@ -7674,7 +7680,7 @@
         <v>220325</v>
       </c>
       <c r="P52" s="28" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="Q52" s="28">
         <v>181083</v>
@@ -7693,7 +7699,7 @@
     </row>
     <row r="53" spans="1:26" ht="15.95">
       <c r="A53" s="37" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B53" s="38">
         <v>326529</v>
@@ -7738,7 +7744,7 @@
         <v>220325</v>
       </c>
       <c r="P53" s="28" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Q53" s="28">
         <v>181084</v>
@@ -7757,7 +7763,7 @@
     </row>
     <row r="54" spans="1:26" ht="15.95">
       <c r="A54" s="37" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="B54" s="38">
         <v>326530</v>
@@ -7802,7 +7808,7 @@
         <v>220325</v>
       </c>
       <c r="P54" s="28" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Q54" s="28">
         <v>181084</v>
@@ -7821,7 +7827,7 @@
     </row>
     <row r="55" spans="1:26" ht="15.95">
       <c r="A55" s="32" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B55" s="33">
         <v>278343</v>
@@ -7864,7 +7870,7 @@
         <v>220325</v>
       </c>
       <c r="P55" s="28" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Q55" s="28">
         <v>181084</v>
@@ -7883,7 +7889,7 @@
     </row>
     <row r="56" spans="1:26" ht="15.95">
       <c r="A56" s="37" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B56" s="38">
         <v>326551</v>
@@ -7926,7 +7932,7 @@
         <v>220325</v>
       </c>
       <c r="P56" s="28" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Q56" s="28">
         <v>181084</v>
@@ -7945,7 +7951,7 @@
     </row>
     <row r="57" spans="1:26" ht="15.95">
       <c r="A57" s="32" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B57" s="33">
         <v>317630</v>
@@ -7988,7 +7994,7 @@
         <v>220325</v>
       </c>
       <c r="P57" s="28" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Q57" s="28">
         <v>181084</v>
@@ -8007,7 +8013,7 @@
     </row>
     <row r="58" spans="1:26" ht="15.95">
       <c r="A58" s="37" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B58" s="38">
         <v>326571</v>
@@ -8050,7 +8056,7 @@
         <v>220325</v>
       </c>
       <c r="P58" s="28" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="Q58" s="28">
         <v>181084</v>
@@ -8069,7 +8075,7 @@
     </row>
     <row r="59" spans="1:26" ht="15.95">
       <c r="A59" s="32" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B59" s="33">
         <v>278344</v>
@@ -8112,7 +8118,7 @@
         <v>220325</v>
       </c>
       <c r="P59" s="28" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Q59" s="28">
         <v>181084</v>
@@ -8131,7 +8137,7 @@
     </row>
     <row r="60" spans="1:26" ht="15.95">
       <c r="A60" s="37" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B60" s="38">
         <v>326552</v>
@@ -8174,7 +8180,7 @@
         <v>220325</v>
       </c>
       <c r="P60" s="28" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Q60" s="28">
         <v>181084</v>
@@ -8193,7 +8199,7 @@
     </row>
     <row r="61" spans="1:26" ht="15.95">
       <c r="A61" s="32" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B61" s="33">
         <v>317631</v>
@@ -8236,7 +8242,7 @@
         <v>220325</v>
       </c>
       <c r="P61" s="28" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Q61" s="28">
         <v>181084</v>
@@ -8255,7 +8261,7 @@
     </row>
     <row r="62" spans="1:26" ht="15.95">
       <c r="A62" s="37" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B62" s="38">
         <v>326572</v>
@@ -8298,7 +8304,7 @@
         <v>220325</v>
       </c>
       <c r="P62" s="28" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="Q62" s="28">
         <v>181084</v>
@@ -8317,7 +8323,7 @@
     </row>
     <row r="63" spans="1:26" ht="15.95">
       <c r="A63" s="37" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B63" s="38">
         <v>326531</v>
@@ -8362,7 +8368,7 @@
         <v>220325</v>
       </c>
       <c r="P63" s="28" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="Q63" s="28">
         <v>181085</v>
@@ -8381,7 +8387,7 @@
     </row>
     <row r="64" spans="1:26" ht="15.95">
       <c r="A64" s="37" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B64" s="38">
         <v>326532</v>
@@ -8426,7 +8432,7 @@
         <v>220325</v>
       </c>
       <c r="P64" s="28" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="Q64" s="28">
         <v>181085</v>
@@ -8445,7 +8451,7 @@
     </row>
     <row r="65" spans="1:26" ht="15.95">
       <c r="A65" s="32" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B65" s="33">
         <v>278345</v>
@@ -8488,7 +8494,7 @@
         <v>220325</v>
       </c>
       <c r="P65" s="28" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="Q65" s="28">
         <v>181085</v>
@@ -8507,7 +8513,7 @@
     </row>
     <row r="66" spans="1:26" ht="15.95">
       <c r="A66" s="37" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B66" s="38">
         <v>326553</v>
@@ -8550,7 +8556,7 @@
         <v>220325</v>
       </c>
       <c r="P66" s="28" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="Q66" s="28">
         <v>181085</v>
@@ -8569,7 +8575,7 @@
     </row>
     <row r="67" spans="1:26" ht="15.95">
       <c r="A67" s="32" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B67" s="33">
         <v>317632</v>
@@ -8612,7 +8618,7 @@
         <v>220325</v>
       </c>
       <c r="P67" s="28" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="Q67" s="28">
         <v>181085</v>
@@ -8631,7 +8637,7 @@
     </row>
     <row r="68" spans="1:26" ht="15.95">
       <c r="A68" s="37" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="B68" s="38">
         <v>326573</v>
@@ -8674,7 +8680,7 @@
         <v>220325</v>
       </c>
       <c r="P68" s="28" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="Q68" s="28">
         <v>181085</v>
@@ -8693,7 +8699,7 @@
     </row>
     <row r="69" spans="1:26" ht="15.95">
       <c r="A69" s="32" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B69" s="33">
         <v>278346</v>
@@ -8736,7 +8742,7 @@
         <v>220325</v>
       </c>
       <c r="P69" s="28" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="Q69" s="28">
         <v>181085</v>
@@ -8755,7 +8761,7 @@
     </row>
     <row r="70" spans="1:26" ht="15.95">
       <c r="A70" s="37" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B70" s="38">
         <v>326554</v>
@@ -8798,7 +8804,7 @@
         <v>220325</v>
       </c>
       <c r="P70" s="28" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="Q70" s="28">
         <v>181085</v>
@@ -8817,7 +8823,7 @@
     </row>
     <row r="71" spans="1:26" ht="15.95">
       <c r="A71" s="32" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B71" s="33">
         <v>317633</v>
@@ -8860,7 +8866,7 @@
         <v>220325</v>
       </c>
       <c r="P71" s="28" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="Q71" s="28">
         <v>181085</v>
@@ -8879,7 +8885,7 @@
     </row>
     <row r="72" spans="1:26" ht="15.95">
       <c r="A72" s="37" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B72" s="38">
         <v>326574</v>
@@ -8922,7 +8928,7 @@
         <v>220325</v>
       </c>
       <c r="P72" s="28" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="Q72" s="28">
         <v>181085</v>
@@ -8941,7 +8947,7 @@
     </row>
     <row r="73" spans="1:26" ht="15.95">
       <c r="A73" s="37" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B73" s="38">
         <v>326533</v>
@@ -8986,7 +8992,7 @@
         <v>220325</v>
       </c>
       <c r="P73" s="28" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="Q73" s="28">
         <v>181086</v>
@@ -9005,7 +9011,7 @@
     </row>
     <row r="74" spans="1:26" ht="15.95">
       <c r="A74" s="37" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B74" s="38">
         <v>326534</v>
@@ -9050,7 +9056,7 @@
         <v>220325</v>
       </c>
       <c r="P74" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="Q74" s="28">
         <v>181086</v>
@@ -9069,7 +9075,7 @@
     </row>
     <row r="75" spans="1:26" ht="15.95">
       <c r="A75" s="37" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B75" s="38">
         <v>326535</v>
@@ -9114,7 +9120,7 @@
         <v>220325</v>
       </c>
       <c r="P75" s="28" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="Q75" s="28">
         <v>181087</v>
@@ -9133,7 +9139,7 @@
     </row>
     <row r="76" spans="1:26" ht="15.95">
       <c r="A76" s="37" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B76" s="38">
         <v>326536</v>
@@ -9178,7 +9184,7 @@
         <v>220325</v>
       </c>
       <c r="P76" s="28" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="Q76" s="28">
         <v>181087</v>
@@ -9197,7 +9203,7 @@
     </row>
     <row r="77" spans="1:26" ht="15.95">
       <c r="A77" s="37" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B77" s="38">
         <v>326537</v>
@@ -9242,7 +9248,7 @@
         <v>220325</v>
       </c>
       <c r="P77" s="28" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="Q77" s="28">
         <v>181088</v>
@@ -9261,7 +9267,7 @@
     </row>
     <row r="78" spans="1:26" ht="15.95">
       <c r="A78" s="37" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B78" s="38">
         <v>326538</v>
@@ -9306,7 +9312,7 @@
         <v>220325</v>
       </c>
       <c r="P78" s="28" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="Q78" s="28">
         <v>181088</v>
@@ -9359,7 +9365,7 @@
         <v>106</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="F1" s="16" t="s">
         <v>112</v>
@@ -9371,13 +9377,13 @@
         <v>124</v>
       </c>
       <c r="I1" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="K1" s="16" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="L1" s="16" t="s">
         <v>142</v>
@@ -9445,10 +9451,10 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="24" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>102</v>
@@ -9460,45 +9466,45 @@
         <v>110</v>
       </c>
       <c r="F3" s="19" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G3" s="20" t="s">
         <v>114</v>
       </c>
       <c r="H3" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I3" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J3" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K3" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L3" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M3" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="O3" s="19" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="P3" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="24" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>102</v>
@@ -9510,45 +9516,45 @@
         <v>110</v>
       </c>
       <c r="F4" s="19" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G4" s="20" t="s">
         <v>116</v>
       </c>
       <c r="H4" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I4" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J4" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K4" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L4" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M4" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="O4" s="19" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P4" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="24" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C5" s="19" t="s">
         <v>102</v>
@@ -9560,45 +9566,45 @@
         <v>110</v>
       </c>
       <c r="F5" s="19" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G5" s="20" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H5" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I5" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J5" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K5" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L5" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M5" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N5" s="21" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="O5" s="19" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="P5" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="24" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="C6" s="19" t="s">
         <v>102</v>
@@ -9610,45 +9616,45 @@
         <v>110</v>
       </c>
       <c r="F6" s="19" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G6" s="20" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H6" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I6" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J6" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K6" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L6" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M6" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="O6" s="19" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="P6" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="24" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C7" s="19" t="s">
         <v>102</v>
@@ -9660,45 +9666,45 @@
         <v>110</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G7" s="20" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H7" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J7" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K7" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L7" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M7" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O7" s="19" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="P7" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="24" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="C8" s="19" t="s">
         <v>102</v>
@@ -9710,45 +9716,45 @@
         <v>110</v>
       </c>
       <c r="F8" s="19" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G8" s="20" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H8" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I8" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J8" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K8" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L8" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M8" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N8" s="20" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O8" s="19" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="P8" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="24" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C9" s="19" t="s">
         <v>102</v>
@@ -9760,45 +9766,45 @@
         <v>110</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H9" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I9" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J9" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K9" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L9" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M9" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="O9" s="19" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="P9" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="24" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="C10" s="19" t="s">
         <v>102</v>
@@ -9810,45 +9816,45 @@
         <v>110</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H10" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I10" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K10" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L10" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M10" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N10" s="20" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="24" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C11" s="19" t="s">
         <v>102</v>
@@ -9860,45 +9866,45 @@
         <v>110</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H11" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I11" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J11" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K11" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L11" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M11" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="O11" s="19" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="P11" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="24" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>102</v>
@@ -9910,45 +9916,45 @@
         <v>110</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H12" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I12" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J12" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K12" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L12" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M12" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="O12" s="19" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="P12" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="24" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C13" s="19" t="s">
         <v>102</v>
@@ -9960,45 +9966,45 @@
         <v>110</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I13" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K13" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L13" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N13" s="21" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="O13" s="19" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="P13" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="24" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C14" s="19" t="s">
         <v>102</v>
@@ -10010,483 +10016,483 @@
         <v>110</v>
       </c>
       <c r="F14" s="19" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G14" s="20" t="s">
         <v>118</v>
       </c>
       <c r="H14" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I14" s="20" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="J14" s="19" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="K14" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L14" s="20" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="M14" s="20" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="N14" s="21" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="O14" s="19" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="P14" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="24" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C15" s="19" t="s">
         <v>104</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E15" s="20" t="s">
         <v>110</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>114</v>
       </c>
       <c r="H15" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I15" s="20" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J15" s="19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="K15" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L15" s="20" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M15" s="20" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N15" s="21" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="O15" s="19" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="P15" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="24" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="C16" s="19" t="s">
         <v>104</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E16" s="20" t="s">
         <v>110</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G16" s="20" t="s">
         <v>116</v>
       </c>
       <c r="H16" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I16" s="20" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J16" s="19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="K16" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L16" s="20" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M16" s="20" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N16" s="21" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="O16" s="19" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="P16" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="24" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C17" s="19" t="s">
         <v>104</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E17" s="20" t="s">
         <v>110</v>
       </c>
       <c r="F17" s="19" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="H17" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I17" s="20" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J17" s="19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="K17" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L17" s="20" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M17" s="20" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N17" s="20" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="O17" s="19" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="P17" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="24" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C18" s="19" t="s">
         <v>104</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E18" s="20" t="s">
         <v>110</v>
       </c>
       <c r="F18" s="19" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="G18" s="20" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="H18" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I18" s="20" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J18" s="19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="K18" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L18" s="20" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M18" s="20" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N18" s="21" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O18" s="19" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="P18" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="24" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C19" s="19" t="s">
         <v>104</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E19" s="20" t="s">
         <v>110</v>
       </c>
       <c r="F19" s="19" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="G19" s="20" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="H19" s="20" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I19" s="20" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="K19" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L19" s="20" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M19" s="20" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N19" s="21" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="O19" s="19" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="P19" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="7" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="C20" s="19" t="s">
         <v>104</v>
       </c>
       <c r="D20" s="19" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E20" s="19" t="s">
         <v>110</v>
       </c>
       <c r="F20" s="19" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G20" s="19" t="s">
         <v>120</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I20" s="19" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J20" s="19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="K20" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L20" s="19" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M20" s="19" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N20" s="19"/>
       <c r="O20" s="19" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="P20" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="7" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="C21" s="19" t="s">
         <v>104</v>
       </c>
       <c r="D21" s="19" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E21" s="19" t="s">
         <v>110</v>
       </c>
       <c r="F21" s="19" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G21" s="19" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="H21" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I21" s="19" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J21" s="19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="K21" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L21" s="19" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M21" s="19" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N21" s="19" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="O21" s="19" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="P21" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="7" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="C22" s="19" t="s">
         <v>104</v>
       </c>
       <c r="D22" s="19" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E22" s="19" t="s">
         <v>110</v>
       </c>
       <c r="F22" s="19" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G22" s="19" t="s">
         <v>122</v>
       </c>
       <c r="H22" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I22" s="19" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J22" s="19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="K22" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L22" s="19" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M22" s="19" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N22" s="19"/>
       <c r="O22" s="19" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="P22" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="7" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="C23" s="19" t="s">
         <v>104</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E23" s="19" t="s">
         <v>110</v>
       </c>
       <c r="F23" s="19" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G23" s="19" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="H23" s="19" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="K23" s="19" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="L23" s="19" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="M23" s="19" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="N23" s="19" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="O23" s="19" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="P23" s="19" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -10513,10 +10519,10 @@
         <v>9</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>138</v>
@@ -10584,10 +10590,10 @@
     </row>
     <row r="2" spans="1:26" ht="32.1">
       <c r="A2" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>145</v>
@@ -10664,7 +10670,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.95">
       <c r="A3" s="6" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="B3" s="1">
         <v>304585</v>
@@ -10862,6 +10868,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e4e246d5-064a-42ac-8fae-0696c9fa62dd">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="ffa00a1b-1412-4262-83a1-58f2742580e0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100B0664017650A5947BA1B6BB62DDE1756" ma:contentTypeVersion="19" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5f9c0f626e79dc52133e521b8706fa1e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e4e246d5-064a-42ac-8fae-0696c9fa62dd" xmlns:ns3="ffa00a1b-1412-4262-83a1-58f2742580e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1f282b496f7fa320b6d535d24d0a2767" ns2:_="" ns3:_="">
     <xsd:import namespace="e4e246d5-064a-42ac-8fae-0696c9fa62dd"/>
@@ -11116,28 +11142,8 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e4e246d5-064a-42ac-8fae-0696c9fa62dd">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="ffa00a1b-1412-4262-83a1-58f2742580e0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67259AB4-4A3F-4792-B9D1-873365319B83}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F8891E3-5751-4A35-B3F5-37B11899C6EA}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11145,7 +11151,7 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F8891E3-5751-4A35-B3F5-37B11899C6EA}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67259AB4-4A3F-4792-B9D1-873365319B83}"/>
 </file>
 
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>